<commit_message>
documentos feitos por todos
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos.xlsx
+++ b/Requisitos/Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PI\grupo9-ads\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B6C10A-B5D0-4D57-9627-592FB5F5AE43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E46CBA-F0E6-47DB-B2A4-259D6057B932}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Descrição</t>
   </si>
@@ -73,21 +73,9 @@
     <t>RF12</t>
   </si>
   <si>
-    <t>RF13</t>
-  </si>
-  <si>
-    <t>RF14</t>
-  </si>
-  <si>
     <t>Projeto Museu</t>
   </si>
   <si>
-    <t>Criar documento de contextualização</t>
-  </si>
-  <si>
-    <t>Criar documento de justificativa</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
@@ -121,12 +109,6 @@
     <t>RNF09</t>
   </si>
   <si>
-    <t>Criar e configurar o projeto no GitHub</t>
-  </si>
-  <si>
-    <t>Alocar os dados de temperatura na plataforma Azure</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
@@ -188,6 +170,18 @@
   </si>
   <si>
     <t xml:space="preserve">Desejável </t>
+  </si>
+  <si>
+    <t>Ter configurado o projeto no GitHub</t>
+  </si>
+  <si>
+    <t>A visualização dos dados deverá ser via web</t>
+  </si>
+  <si>
+    <t>Dados de temperatura e umidade deverão ser alocados na plataforma Azure</t>
+  </si>
+  <si>
+    <t>Ter api que controla a temperatura e umidade das geladeiras</t>
   </si>
 </sst>
 </file>
@@ -322,25 +316,25 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Ênfase1" xfId="1" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -373,26 +367,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -413,21 +387,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -707,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,15 +685,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -764,161 +728,154 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6" t="s">
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>47</v>
+      <c r="C14" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
     </row>
@@ -953,14 +910,10 @@
       <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -970,43 +923,37 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C30:C35 C3:C25">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="C28:C33 C3:C23">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C35 C2:C25" xr:uid="{D1C3E77C-7649-4BAF-936B-1CC1A2AF9EA0}">
-      <formula1>$F$1:$F$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C33 C2:C23" xr:uid="{D1C3E77C-7649-4BAF-936B-1CC1A2AF9EA0}">
+      <formula1>$F$1:$F$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1019,7 +966,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,124 +978,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>20</v>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10" xr:uid="{04C0F63B-1635-442D-94B6-997633ED140B}">
+      <formula1>$E$1:$E$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>